<commit_message>
Update Hs database (REF correction)
</commit_message>
<xml_diff>
--- a/ecosysem/db/Excels/Hs.xlsx
+++ b/ecosysem/db/Excels/Hs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2424069M\Documents\GitHub\EcoSysEM\ecosysem\db\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438A3E8E-6B13-48D5-96FB-D0DBDE248447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED2E802-8513-418D-83CC-60EB25862691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{A13132EB-A149-4D8F-BD03-0192B745A142}"/>
+    <workbookView xWindow="-11520" yWindow="600" windowWidth="11520" windowHeight="12360" xr2:uid="{A13132EB-A149-4D8F-BD03-0192B745A142}"/>
   </bookViews>
   <sheets>
     <sheet name="Hs" sheetId="1" r:id="rId1"/>
@@ -212,7 +212,7 @@
     <t>H2S</t>
   </si>
   <si>
-    <t>Douabul2005</t>
+    <t>Douabul1979b</t>
   </si>
 </sst>
 </file>
@@ -619,8 +619,8 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>